<commit_message>
Was created code for building charts about energy and electricity consuption
</commit_message>
<xml_diff>
--- a/Total Electricity Consumption.xlsx
+++ b/Total Electricity Consumption.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dmitrii/Desktop/PhD/Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Никита\Desktop\Новая папка (2)\Vasenin_charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340DE086-2AA2-0C41-BE22-2118B0DAEE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="1600" windowWidth="13440" windowHeight="11880" xr2:uid="{2AC084D7-1D63-054B-88D5-9C36A4D630D9}"/>
+    <workbookView xWindow="1343" yWindow="1598" windowWidth="13440" windowHeight="11880" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="World" sheetId="1" r:id="rId1"/>
     <sheet name="Europe" sheetId="2" r:id="rId2"/>
     <sheet name="Italy" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,18 +42,6 @@
     <t>i</t>
   </si>
   <si>
-    <t>TEC, G, I, TJ</t>
-  </si>
-  <si>
-    <t>TEC, R, I, TJ</t>
-  </si>
-  <si>
-    <t>∆% TEC, G</t>
-  </si>
-  <si>
-    <t>∆% TEC, R</t>
-  </si>
-  <si>
     <t>0.00%</t>
   </si>
   <si>
@@ -164,12 +151,24 @@
   </si>
   <si>
     <t>149.85%</t>
+  </si>
+  <si>
+    <t>TEC,G,I,TJ</t>
+  </si>
+  <si>
+    <t>TEC,R,I,TJ</t>
+  </si>
+  <si>
+    <t>∆%TEC,G</t>
+  </si>
+  <si>
+    <t>∆%TEC,R</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -257,8 +256,8 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Per cent" xfId="1" builtinId="5"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Процентный" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -275,6 +274,50 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
         <vertical/>
         <horizontal style="thin">
           <color auto="1"/>
@@ -295,6 +338,116 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
         <vertical/>
         <horizontal style="thin">
           <color auto="1"/>
@@ -315,271 +468,117 @@
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color auto="1"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
         <vertical/>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color auto="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
         <horizontal style="thin">
           <color auto="1"/>
         </horizontal>
@@ -665,45 +664,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BF1F1E71-2A96-EE40-9C8A-B32091ADC0A3}" name="Table13" displayName="Table13" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8" xr:uid="{BF1F1E71-2A96-EE40-9C8A-B32091ADC0A3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table13" displayName="Table13" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A2109B12-B560-F348-B7AB-9452F936E8BC}" name="Year" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{7631CA42-A810-824C-80BA-7F6219AF8E06}" name="i" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{2586F6AE-5578-2F48-9C8C-90D7CE709BC5}" name="TEC, G, I, TJ" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{4445289F-6BC1-B148-B091-9BC694C37E54}" name="TEC, R, I, TJ" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{0D796778-72B4-4347-B888-865FC594FE6A}" name="∆% TEC, G" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{D767771D-0C4A-B740-B84A-12E14C129F27}" name="∆% TEC, R" dataDxfId="6"/>
+    <tableColumn id="1" name="Year" dataDxfId="17"/>
+    <tableColumn id="2" name="i" dataDxfId="16"/>
+    <tableColumn id="3" name="TEC,G,I,TJ" dataDxfId="15"/>
+    <tableColumn id="4" name="TEC,R,I,TJ" dataDxfId="14"/>
+    <tableColumn id="5" name="∆%TEC,G" dataDxfId="13"/>
+    <tableColumn id="6" name="∆%TEC,R" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{9C7A21E4-D53E-3643-A2E6-1F8DAA1EE683}" name="Table133" displayName="Table133" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8" xr:uid="{9C7A21E4-D53E-3643-A2E6-1F8DAA1EE683}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table133" displayName="Table133" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C2772FD5-94FE-7A4E-8ADA-BCCDE642B86F}" name="Year" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{93162949-0ABF-F84E-8BC6-AEDD814F6DF1}" name="i" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{429B00D5-CFB5-134C-BAD9-679E3EE606D8}" name="TEC, G, I, TJ" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{3F8BC056-2833-EF4F-85B9-0B3B6D784FE8}" name="TEC, R, I, TJ" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{75070282-76B7-F04C-ACDA-DFCBC4F6FB1B}" name="∆% TEC, G" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{F78A6F86-0E13-E24D-97C6-4B596FC05D3A}" name="∆% TEC, R" dataDxfId="13"/>
+    <tableColumn id="1" name="Year" dataDxfId="11"/>
+    <tableColumn id="2" name="i" dataDxfId="10"/>
+    <tableColumn id="3" name="TEC,G,I,TJ" dataDxfId="9"/>
+    <tableColumn id="4" name="TEC,R,I,TJ" dataDxfId="8"/>
+    <tableColumn id="5" name="∆%TEC,G" dataDxfId="7"/>
+    <tableColumn id="6" name="∆%TEC,R" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{539654CE-6BDE-0A45-8ED6-000661752213}" name="Table134" displayName="Table134" ref="A1:F8" totalsRowShown="0">
-  <autoFilter ref="A1:F8" xr:uid="{539654CE-6BDE-0A45-8ED6-000661752213}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A1:F8" totalsRowShown="0">
+  <autoFilter ref="A1:F8"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{82356DE9-4FBC-714F-9A01-58FDD0D0EBBD}" name="Year" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{C8B07A28-F531-EA49-8CD4-8DCA7706BD1C}" name="i" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{0CE0B8E4-8DEC-6F40-B3B6-3A49CDDD6F88}" name="TEC, G, I, TJ" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{F0B76AA0-0DF9-6647-8BFF-703EEE594CA8}" name="TEC, R, I, TJ" dataDxfId="0"/>
-    <tableColumn id="5" xr3:uid="{F536351E-1C2B-244E-9121-87B6F57890A9}" name="∆% TEC, G" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{0DAEB227-3B41-5B48-B5A0-CFD85497E777}" name="∆% TEC, R" dataDxfId="8"/>
+    <tableColumn id="1" name="Year" dataDxfId="5"/>
+    <tableColumn id="2" name="i" dataDxfId="4"/>
+    <tableColumn id="3" name="TEC,G,I,TJ" dataDxfId="3"/>
+    <tableColumn id="4" name="TEC,R,I,TJ" dataDxfId="2"/>
+    <tableColumn id="5" name="∆%TEC,G" dataDxfId="1"/>
+    <tableColumn id="6" name="∆%TEC,R" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1005,22 +1004,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41845F93-E795-8A46-AA19-C2B2CBA65C81}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="12.8125" customWidth="1"/>
+    <col min="5" max="5" width="12.3125" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1028,19 +1027,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>1990</v>
       </c>
@@ -1054,13 +1053,13 @@
         <v>9053247</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1995</v>
       </c>
@@ -1074,13 +1073,13 @@
         <v>11010488</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>2000</v>
       </c>
@@ -1094,13 +1093,13 @@
         <v>12824710</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -1114,13 +1113,13 @@
         <v>15151447</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>2010</v>
       </c>
@@ -1134,13 +1133,13 @@
         <v>17899811</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -1154,13 +1153,13 @@
         <v>19784593</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>2020</v>
       </c>
@@ -1174,10 +1173,10 @@
         <v>22619944</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1190,21 +1189,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A1C3C0-C8A6-5748-ADB6-DFF0611167AD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.3125" customWidth="1"/>
+    <col min="4" max="4" width="13.8125" customWidth="1"/>
+    <col min="5" max="5" width="12.6875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1212,19 +1211,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>1990</v>
       </c>
@@ -1238,13 +1237,13 @@
         <v>2537955</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1995</v>
       </c>
@@ -1258,13 +1257,13 @@
         <v>2856091</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>2000</v>
       </c>
@@ -1278,13 +1277,13 @@
         <v>3121142</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -1298,13 +1297,13 @@
         <v>3428698</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>2010</v>
       </c>
@@ -1318,13 +1317,13 @@
         <v>3736802</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -1338,13 +1337,13 @@
         <v>3593569</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>2020</v>
       </c>
@@ -1358,10 +1357,10 @@
         <v>3732327</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -1373,22 +1372,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE71CD7F-0211-414E-AA96-CA0B34E73901}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="3" max="3" width="13.5" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" customWidth="1"/>
+    <col min="6" max="6" width="12.1875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1396,19 +1395,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A2" s="1">
         <v>1990</v>
       </c>
@@ -1422,13 +1421,13 @@
         <v>189828</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A3" s="1">
         <v>1995</v>
       </c>
@@ -1442,13 +1441,13 @@
         <v>206078</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A4" s="1">
         <v>2000</v>
       </c>
@@ -1462,13 +1461,13 @@
         <v>220003</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A5" s="1">
         <v>2005</v>
       </c>
@@ -1482,13 +1481,13 @@
         <v>241056</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A6" s="1">
         <v>2010</v>
       </c>
@@ -1502,13 +1501,13 @@
         <v>250380</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A7" s="1">
         <v>2015</v>
       </c>
@@ -1522,13 +1521,13 @@
         <v>238273</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.5">
       <c r="A8" s="1">
         <v>2020</v>
       </c>
@@ -1542,10 +1541,10 @@
         <v>238362</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>